<commit_message>
added optional opac request to read header plugin
</commit_message>
<xml_diff>
--- a/goobi-plugin-import-excel/sample-for-header-import.xlsx
+++ b/goobi-plugin-import-excel/sample-for-header-import.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="38">
-  <si>
-    <t xml:space="preserve">1-PPN-Digital</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+  <si>
+    <t xml:space="preserve">PPN-A</t>
   </si>
   <si>
     <t xml:space="preserve">2-Titel</t>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">8-Jahr</t>
   </si>
   <si>
-    <t xml:space="preserve">9-PPN-Orig</t>
+    <t xml:space="preserve">PPN-O</t>
   </si>
   <si>
     <t xml:space="preserve">10-DocLanguage</t>
@@ -55,95 +55,60 @@
     <t xml:space="preserve">11-Person</t>
   </si>
   <si>
+    <t xml:space="preserve">867383437</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slawistik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Greifswald</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4021965-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Helene</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Anden</t>
+  </si>
+  <si>
     <t xml:space="preserve">PPN33230</t>
   </si>
   <si>
-    <t xml:space="preserve">Slawistik</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Greifswald</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4021965-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Helene</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anden</t>
-  </si>
-  <si>
     <t xml:space="preserve">ger</t>
   </si>
   <si>
     <t xml:space="preserve">Anden, Helene</t>
   </si>
   <si>
+    <t xml:space="preserve">868963453</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deutsch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blühm</t>
+  </si>
+  <si>
     <t xml:space="preserve">PPN33231</t>
   </si>
   <si>
-    <t xml:space="preserve">Deutsch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Blühm</t>
-  </si>
-  <si>
     <t xml:space="preserve">Blühm, Elger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PPN33232</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geschichte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ruth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bork</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bork, Ruth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PPN33233</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Anglistik</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rolf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Berndt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Berndt, Rolf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PPN33234</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Wolfgang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brüske</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Brüske, Wolfgang</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -165,6 +130,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -236,17 +208,21 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -271,7 +247,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -315,7 +291,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
@@ -324,7 +300,7 @@
       <c r="C2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="0" t="s">
@@ -340,144 +316,71 @@
         <v>1955</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>19</v>
+      <c r="A3" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H3" s="0" t="n">
         <v>1950</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="0" t="n">
-        <v>1951</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>28</v>
-      </c>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="0" t="n">
-        <v>1951</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="0" t="s">
-        <v>33</v>
-      </c>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="H6" s="0" t="n">
-        <v>1952</v>
-      </c>
-      <c r="I6" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>37</v>
-      </c>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>